<commit_message>
Correción Sprint y BD
</commit_message>
<xml_diff>
--- a/SCRUM/Sprints.xlsx
+++ b/SCRUM/Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreye\Documents\TecNMCampusCuliacan\Git Repositories\Sistema-Incidencias\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1B7D55-4F94-4ED6-8B24-E30D211AE57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C661D8-1D37-4FFC-9DE7-E094D614F067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C2CACDC-A4BC-4DCF-8181-CE8927475787}"/>
   </bookViews>
@@ -132,16 +132,16 @@
     <t>Agregar dispositivos</t>
   </si>
   <si>
-    <t>Agregar Departamentos Tecnico</t>
-  </si>
-  <si>
-    <t>Asignar departamento Jefe Departamento</t>
-  </si>
-  <si>
     <t>Manuel Ramirez y Felipe Saille</t>
   </si>
   <si>
     <t>2    20/10/2020</t>
+  </si>
+  <si>
+    <t>Modificar Jefe Departamento (Jefe)</t>
+  </si>
+  <si>
+    <t>Modificar Tecnico (Técnico)</t>
   </si>
 </sst>
 </file>
@@ -263,47 +263,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,7 +622,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K14"/>
+      <selection activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,46 +633,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="16" t="s">
+      <c r="K2" s="16"/>
+      <c r="L2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -680,22 +680,22 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="6">
+      <c r="F3" s="10">
         <v>44109</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6">
+      <c r="G3" s="11"/>
+      <c r="H3" s="10">
         <v>44116</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="8">
         <v>7</v>
       </c>
@@ -706,22 +706,22 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="6">
+      <c r="F4" s="10">
         <v>44109</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6">
+      <c r="G4" s="11"/>
+      <c r="H4" s="10">
         <v>44116</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="8">
         <v>7</v>
       </c>
@@ -732,19 +732,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="6">
+      <c r="F5" s="10">
         <v>44109</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6">
+      <c r="G5" s="11"/>
+      <c r="H5" s="10">
         <v>44116</v>
       </c>
       <c r="I5" s="9"/>
@@ -758,26 +758,26 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="15">
         <v>44116</v>
       </c>
       <c r="G6" s="15"/>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13">
         <v>2</v>
       </c>
-      <c r="K6" s="14"/>
+      <c r="K6" s="13"/>
       <c r="L6" s="1" t="s">
         <v>16</v>
       </c>
@@ -792,10 +792,10 @@
         <v>17</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="8" t="s">
         <v>20</v>
       </c>
@@ -814,14 +814,14 @@
         <v>30</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="8" t="s">
         <v>20</v>
       </c>
@@ -835,36 +835,36 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="6">
+      <c r="F10" s="10">
         <v>44124</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6">
+      <c r="G10" s="11"/>
+      <c r="H10" s="10">
         <v>44137</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="8">
         <v>7</v>
       </c>
@@ -875,22 +875,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="6">
+      <c r="F11" s="10">
         <v>44125</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6">
+      <c r="G11" s="11"/>
+      <c r="H11" s="10">
         <v>44138</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="8">
         <v>7</v>
       </c>
@@ -901,127 +901,183 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="12"/>
       <c r="D12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
         <v>44126</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6">
+      <c r="G12" s="11"/>
+      <c r="H12" s="10">
         <v>44139</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="14">
+      <c r="I12" s="11"/>
+      <c r="J12" s="13">
         <v>7</v>
       </c>
-      <c r="K12" s="14"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
@@ -1036,67 +1092,11 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>